<commit_message>
updated numbers and diags
</commit_message>
<xml_diff>
--- a/Results/pipeline.xlsx
+++ b/Results/pipeline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,15 +96,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,7 +395,7 @@
   <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -385,7 +413,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>13467548</v>
+        <v>17686161</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -399,11 +427,11 @@
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>3725106</v>
+        <v>5562533</v>
       </c>
       <c r="D3" s="1">
         <f>C3/C2</f>
-        <v>0.2765986800269804</v>
+        <v>0.31451330789084186</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -414,11 +442,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>581435</v>
+        <v>918988</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:D8" si="0">C4/C3</f>
-        <v>0.15608549125850379</v>
+        <v>0.16521034571839843</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -429,11 +457,11 @@
         <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>412623</v>
+        <v>756588</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>0.70966316097242166</v>
+        <v>0.82328387313000828</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -444,11 +472,11 @@
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>31666</v>
+        <v>44735</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>7.6743177185954248E-2</v>
+        <v>5.912729252909113E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -459,11 +487,11 @@
         <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>31666</v>
+        <v>38989</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.87155471107633842</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -474,11 +502,11 @@
         <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>289</v>
+        <v>433</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>9.1265079264826621E-3</v>
+        <v>1.1105696478493934E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>